<commit_message>
output file from scenario analysis
</commit_message>
<xml_diff>
--- a/output/demographic_walkshed_quarter_mi_bg.xlsx
+++ b/output/demographic_walkshed_quarter_mi_bg.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://perkinswillinc-my.sharepoint.com/personal/ykweon_nelsonnygaard_com/Documents/Documents/github/NN/R/woodburn-transit/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="11_A676902300996FCD3C0429FA5F3D0152EA5D599A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44BAAA61-56F7-4F5A-BFAC-9C932617A6BE}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="11_A676902300996FCD3C0429FA5F3D0152EA5D599A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8EB55400-230C-4495-9A1B-C6A121D52835}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="3816" yWindow="2196" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="demographic_bg" sheetId="1" r:id="rId1"/>
@@ -487,12 +487,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.5546875" customWidth="1"/>
+    <col min="4" max="4" width="26.88671875" customWidth="1"/>
+    <col min="5" max="5" width="21.5546875" customWidth="1"/>
+    <col min="6" max="6" width="22.5546875" customWidth="1"/>
+    <col min="7" max="7" width="29.21875" customWidth="1"/>
     <col min="11" max="11" width="34.21875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1171,8 +1177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FB479B1-92E0-4269-AEC7-3D3233F06D85}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>